<commit_message>
processed statuses and reprocess analyses and datafiles
</commit_message>
<xml_diff>
--- a/localExperiments/hazardIdentification/hazardIdentification.xlsx
+++ b/localExperiments/hazardIdentification/hazardIdentification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattsears/code/eyetracker/localExperiments/hazardIdentification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34FB962E-6884-284A-AEA7-2191D99C8A16}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96094CB-E6DE-444E-BE6D-96A3CB134A0C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="9560" xr2:uid="{3006803E-C1FE-6049-930A-55B4D31C99D5}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19000" xr2:uid="{3006803E-C1FE-6049-930A-55B4D31C99D5}"/>
   </bookViews>
   <sheets>
     <sheet name="hazardIdentification" sheetId="1" r:id="rId1"/>
@@ -431,12 +431,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -506,6 +500,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -824,7 +824,7 @@
   <dimension ref="A1:W32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+      <selection activeCell="S30" sqref="S30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -958,31 +958,31 @@
         <v>0</v>
       </c>
       <c r="N2" s="3">
-        <f>D2</f>
+        <f t="shared" ref="N2:N19" si="0">D2</f>
         <v>1</v>
       </c>
       <c r="O2" s="3">
-        <f>N2</f>
+        <f t="shared" ref="O2:O19" si="1">N2</f>
         <v>1</v>
       </c>
       <c r="P2" s="3">
-        <f>E2</f>
+        <f t="shared" ref="P2:P19" si="2">E2</f>
         <v>1</v>
       </c>
       <c r="Q2" s="3">
-        <f>P2</f>
+        <f t="shared" ref="Q2:Q19" si="3">P2</f>
         <v>1</v>
       </c>
       <c r="R2" s="3">
-        <f>SUM(F2:M2)</f>
+        <f t="shared" ref="R2:R19" si="4">SUM(F2:M2)</f>
         <v>1</v>
       </c>
       <c r="S2" s="3">
-        <f>R2/8</f>
+        <f t="shared" ref="S2:S19" si="5">R2/8</f>
         <v>0.125</v>
       </c>
       <c r="T2" s="3">
-        <f>N2+P2+R2</f>
+        <f t="shared" ref="T2:T19" si="6">N2+P2+R2</f>
         <v>3</v>
       </c>
       <c r="U2" s="3">
@@ -993,7 +993,7 @@
         <v>87607</v>
       </c>
       <c r="W2" s="3">
-        <f>T2/V2*1000</f>
+        <f t="shared" ref="W2:W19" si="7">T2/V2*1000</f>
         <v>3.4243838962639973E-2</v>
       </c>
     </row>
@@ -1038,31 +1038,31 @@
         <v>0</v>
       </c>
       <c r="N3" s="3">
-        <f>D3</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O3" s="3">
-        <f>N3</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P3" s="3">
-        <f>E3</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Q3" s="3">
-        <f>P3</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="R3" s="3">
-        <f>SUM(F3:M3)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="S3" s="3">
-        <f>R3/8</f>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="T3" s="3">
-        <f>N3+P3+R3</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="U3" s="3">
@@ -1073,7 +1073,7 @@
         <v>129725</v>
       </c>
       <c r="W3" s="3">
-        <f>T3/V3*1000</f>
+        <f t="shared" si="7"/>
         <v>4.6251686259394874E-2</v>
       </c>
     </row>
@@ -1118,31 +1118,31 @@
         <v>0</v>
       </c>
       <c r="N4" s="3">
-        <f>D4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O4" s="3">
-        <f>N4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P4" s="3">
-        <f>E4</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Q4" s="3">
-        <f>P4</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="R4" s="3">
-        <f>SUM(F4:M4)</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="S4" s="3">
-        <f>R4/8</f>
+        <f t="shared" si="5"/>
         <v>0.625</v>
       </c>
       <c r="T4" s="3">
-        <f>N4+P4+R4</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="U4" s="3">
@@ -1153,7 +1153,7 @@
         <v>85085</v>
       </c>
       <c r="W4" s="3">
-        <f>T4/V4*1000</f>
+        <f t="shared" si="7"/>
         <v>7.05177175765411E-2</v>
       </c>
     </row>
@@ -1198,31 +1198,31 @@
         <v>1</v>
       </c>
       <c r="N5" s="3">
-        <f>D5</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O5" s="3">
-        <f>N5</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P5" s="3">
-        <f>E5</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q5" s="3">
-        <f>P5</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R5" s="3">
-        <f>SUM(F5:M5)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="S5" s="3">
-        <f>R5/8</f>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="T5" s="3">
-        <f>N5+P5+R5</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="U5" s="3">
@@ -1233,7 +1233,7 @@
         <v>72289</v>
       </c>
       <c r="W5" s="3">
-        <f>T5/V5*1000</f>
+        <f t="shared" si="7"/>
         <v>5.5333453222481982E-2</v>
       </c>
     </row>
@@ -1278,31 +1278,31 @@
         <v>1</v>
       </c>
       <c r="N6" s="3">
-        <f>D6</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O6" s="3">
-        <f>N6</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P6" s="3">
-        <f>E6</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Q6" s="3">
-        <f>P6</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="R6" s="3">
-        <f>SUM(F6:M6)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="S6" s="3">
-        <f>R6/8</f>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="T6" s="3">
-        <f>N6+P6+R6</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="U6" s="3">
@@ -1313,7 +1313,7 @@
         <v>97165</v>
       </c>
       <c r="W6" s="3">
-        <f>T6/V6*1000</f>
+        <f t="shared" si="7"/>
         <v>6.1750630371018377E-2</v>
       </c>
     </row>
@@ -1358,31 +1358,31 @@
         <v>0</v>
       </c>
       <c r="N7" s="3">
-        <f>D7</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O7" s="3">
-        <f>N7</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P7" s="3">
-        <f>E7</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Q7" s="3">
-        <f>P7</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="R7" s="3">
-        <f>SUM(F7:M7)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="S7" s="3">
-        <f>R7/8</f>
+        <f t="shared" si="5"/>
         <v>0.375</v>
       </c>
       <c r="T7" s="3">
-        <f>N7+P7+R7</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="U7" s="3">
@@ -1393,7 +1393,7 @@
         <v>60706</v>
       </c>
       <c r="W7" s="3">
-        <f>T7/V7*1000</f>
+        <f t="shared" si="7"/>
         <v>6.5891345171811694E-2</v>
       </c>
     </row>
@@ -1438,31 +1438,31 @@
         <v>0</v>
       </c>
       <c r="N8" s="3">
-        <f>D8</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O8" s="3">
-        <f>N8</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P8" s="3">
-        <f>E8</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Q8" s="3">
-        <f>P8</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="R8" s="3">
-        <f>SUM(F8:M8)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="S8" s="3">
-        <f>R8/8</f>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="T8" s="3">
-        <f>N8+P8+R8</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="U8" s="3">
@@ -1473,7 +1473,7 @@
         <v>97978</v>
       </c>
       <c r="W8" s="3">
-        <f>T8/V8*1000</f>
+        <f t="shared" si="7"/>
         <v>6.1238237155279762E-2</v>
       </c>
     </row>
@@ -1518,31 +1518,31 @@
         <v>0</v>
       </c>
       <c r="N9" s="3">
-        <f>D9</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O9" s="3">
-        <f>N9</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P9" s="3">
-        <f>E9</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Q9" s="3">
-        <f>P9</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="R9" s="3">
-        <f>SUM(F9:M9)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="S9" s="3">
-        <f>R9/8</f>
+        <f t="shared" si="5"/>
         <v>0.25</v>
       </c>
       <c r="T9" s="3">
-        <f>N9+P9+R9</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="U9" s="3">
@@ -1553,7 +1553,7 @@
         <v>34269</v>
       </c>
       <c r="W9" s="3">
-        <f>T9/V9*1000</f>
+        <f t="shared" si="7"/>
         <v>0.11672356940675246</v>
       </c>
     </row>
@@ -1598,31 +1598,31 @@
         <v>0</v>
       </c>
       <c r="N10" s="3">
-        <f>D10</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O10" s="3">
-        <f>N10</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P10" s="3">
-        <f>E10</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Q10" s="3">
-        <f>P10</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="R10" s="3">
-        <f>SUM(F10:M10)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="S10" s="3">
-        <f>R10/8</f>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="T10" s="3">
-        <f>N10+P10+R10</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="U10" s="3">
@@ -1633,7 +1633,7 @@
         <v>52640</v>
       </c>
       <c r="W10" s="3">
-        <f>T10/V10*1000</f>
+        <f t="shared" si="7"/>
         <v>0.11398176291793312</v>
       </c>
     </row>
@@ -1678,31 +1678,31 @@
         <v>0</v>
       </c>
       <c r="N11" s="3">
-        <f>D11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O11" s="3">
-        <f>N11</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P11" s="3">
-        <f>E11</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Q11" s="3">
-        <f>P11</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="R11" s="3">
-        <f>SUM(F11:M11)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="S11" s="3">
-        <f>R11/8</f>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="T11" s="3">
-        <f>N11+P11+R11</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="U11" s="3">
@@ -1713,7 +1713,7 @@
         <v>72040</v>
       </c>
       <c r="W11" s="3">
-        <f>T11/V11*1000</f>
+        <f t="shared" si="7"/>
         <v>6.9405885619100507E-2</v>
       </c>
     </row>
@@ -1758,31 +1758,31 @@
         <v>0</v>
       </c>
       <c r="N12" s="3">
-        <f>D12</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O12" s="3">
-        <f>N12</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P12" s="3">
-        <f>E12</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Q12" s="3">
-        <f>P12</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="R12" s="3">
-        <f>SUM(F12:M12)</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="S12" s="3">
-        <f>R12/8</f>
+        <f t="shared" si="5"/>
         <v>0.625</v>
       </c>
       <c r="T12" s="3">
-        <f>N12+P12+R12</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="U12" s="3">
@@ -1793,7 +1793,7 @@
         <v>122955</v>
       </c>
       <c r="W12" s="3">
-        <f>T12/V12*1000</f>
+        <f t="shared" si="7"/>
         <v>5.6931397665812691E-2</v>
       </c>
     </row>
@@ -1838,31 +1838,31 @@
         <v>0</v>
       </c>
       <c r="N13" s="3">
-        <f>D13</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O13" s="3">
-        <f>N13</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P13" s="3">
-        <f>E13</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Q13" s="3">
-        <f>P13</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="R13" s="3">
-        <f>SUM(F13:M13)</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="S13" s="3">
-        <f>R13/8</f>
+        <f t="shared" si="5"/>
         <v>0.875</v>
       </c>
       <c r="T13" s="3">
-        <f>N13+P13+R13</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="U13" s="3">
@@ -1873,7 +1873,7 @@
         <v>125311</v>
       </c>
       <c r="W13" s="3">
-        <f>T13/V13*1000</f>
+        <f t="shared" si="7"/>
         <v>7.1821308584242405E-2</v>
       </c>
     </row>
@@ -1918,31 +1918,31 @@
         <v>0</v>
       </c>
       <c r="N14" s="3">
-        <f>D14</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O14" s="3">
-        <f>N14</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P14" s="3">
-        <f>E14</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q14" s="3">
-        <f>P14</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R14" s="3">
-        <f>SUM(F14:M14)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="S14" s="3">
-        <f>R14/8</f>
+        <f t="shared" si="5"/>
         <v>0.375</v>
       </c>
       <c r="T14" s="3">
-        <f>N14+P14+R14</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="U14" s="3">
@@ -1953,7 +1953,7 @@
         <v>69219</v>
       </c>
       <c r="W14" s="3">
-        <f>T14/V14*1000</f>
+        <f t="shared" si="7"/>
         <v>5.7787601670061688E-2</v>
       </c>
     </row>
@@ -1998,31 +1998,31 @@
         <v>0</v>
       </c>
       <c r="N15" s="3">
-        <f>D15</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O15" s="3">
-        <f>N15</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P15" s="3">
-        <f>E15</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Q15" s="3">
-        <f>P15</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="R15" s="3">
-        <f>SUM(F15:M15)</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="S15" s="3">
-        <f>R15/8</f>
+        <f t="shared" si="5"/>
         <v>0.75</v>
       </c>
       <c r="T15" s="3">
-        <f>N15+P15+R15</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="U15" s="3">
@@ -2033,7 +2033,7 @@
         <v>104567</v>
       </c>
       <c r="W15" s="3">
-        <f>T15/V15*1000</f>
+        <f t="shared" si="7"/>
         <v>7.6505972247458573E-2</v>
       </c>
     </row>
@@ -2078,31 +2078,31 @@
         <v>0</v>
       </c>
       <c r="N16" s="3">
-        <f>D16</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O16" s="3">
-        <f>N16</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P16" s="3">
-        <f>E16</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Q16" s="3">
-        <f>P16</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="R16" s="3">
-        <f>SUM(F16:M16)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="S16" s="3">
-        <f>R16/8</f>
+        <f t="shared" si="5"/>
         <v>0.375</v>
       </c>
       <c r="T16" s="3">
-        <f>N16+P16+R16</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="U16" s="3">
@@ -2113,7 +2113,7 @@
         <v>46135</v>
       </c>
       <c r="W16" s="3">
-        <f>T16/V16*1000</f>
+        <f t="shared" si="7"/>
         <v>8.6702070011921539E-2</v>
       </c>
     </row>
@@ -2158,31 +2158,31 @@
         <v>0</v>
       </c>
       <c r="N17" s="3">
-        <f>D17</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O17" s="3">
-        <f>N17</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P17" s="3">
-        <f>E17</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Q17" s="3">
-        <f>P17</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="R17" s="3">
-        <f>SUM(F17:M17)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="S17" s="3">
-        <f>R17/8</f>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="T17" s="3">
-        <f>N17+P17+R17</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="U17" s="3">
@@ -2193,7 +2193,7 @@
         <v>54748</v>
       </c>
       <c r="W17" s="3">
-        <f>T17/V17*1000</f>
+        <f t="shared" si="7"/>
         <v>9.1327537078980059E-2</v>
       </c>
     </row>
@@ -2238,31 +2238,31 @@
         <v>0</v>
       </c>
       <c r="N18" s="3">
-        <f>D18</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O18" s="3">
-        <f>N18</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P18" s="3">
-        <f>E18</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Q18" s="3">
-        <f>P18</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="R18" s="3">
-        <f>SUM(F18:M18)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="S18" s="3">
-        <f>R18/8</f>
+        <f t="shared" si="5"/>
         <v>0.375</v>
       </c>
       <c r="T18" s="3">
-        <f>N18+P18+R18</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="U18" s="3">
@@ -2273,7 +2273,7 @@
         <v>69850</v>
       </c>
       <c r="W18" s="3">
-        <f>T18/V18*1000</f>
+        <f t="shared" si="7"/>
         <v>7.158196134574088E-2</v>
       </c>
     </row>
@@ -2318,31 +2318,31 @@
         <v>0</v>
       </c>
       <c r="N19" s="3">
-        <f>D19</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O19" s="3">
-        <f>N19</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P19" s="3">
-        <f>E19</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Q19" s="3">
-        <f>P19</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="R19" s="3">
-        <f>SUM(F19:M19)</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="S19" s="3">
-        <f>R19/8</f>
+        <f t="shared" si="5"/>
         <v>0.625</v>
       </c>
       <c r="T19" s="3">
-        <f>N19+P19+R19</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="U19" s="3">
@@ -2353,7 +2353,7 @@
         <v>79989</v>
       </c>
       <c r="W19" s="3">
-        <f>T19/V19*1000</f>
+        <f t="shared" si="7"/>
         <v>8.7512032904524376E-2</v>
       </c>
     </row>
@@ -2381,19 +2381,19 @@
       <c r="W21" s="2"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A25" s="31"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="31"/>
-      <c r="L25" s="31"/>
-      <c r="M25" s="31"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="29"/>
       <c r="N25"/>
       <c r="O25"/>
       <c r="P25"/>
@@ -2404,19 +2404,19 @@
       <c r="U25"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A26" s="31"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="31"/>
-      <c r="J26" s="31"/>
-      <c r="K26" s="31"/>
-      <c r="L26" s="31"/>
-      <c r="M26" s="31"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="29"/>
       <c r="N26"/>
       <c r="O26"/>
       <c r="P26"/>
@@ -2427,19 +2427,19 @@
       <c r="U26"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A27" s="31"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="31"/>
-      <c r="L27" s="31"/>
-      <c r="M27" s="31"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="29"/>
+      <c r="M27" s="29"/>
       <c r="N27"/>
       <c r="O27"/>
       <c r="P27"/>
@@ -2450,19 +2450,19 @@
       <c r="U27"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A28" s="31"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
-      <c r="K28" s="31"/>
-      <c r="L28" s="31"/>
-      <c r="M28" s="31"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="29"/>
+      <c r="L28" s="29"/>
+      <c r="M28" s="29"/>
       <c r="N28"/>
       <c r="O28"/>
       <c r="P28"/>
@@ -2473,19 +2473,19 @@
       <c r="U28"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A29" s="31"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="31"/>
-      <c r="K29" s="31"/>
-      <c r="L29" s="31"/>
-      <c r="M29" s="31"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="29"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="29"/>
       <c r="N29"/>
       <c r="O29"/>
       <c r="P29"/>
@@ -2496,19 +2496,19 @@
       <c r="U29"/>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A30" s="31"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
-      <c r="K30" s="31"/>
-      <c r="L30" s="31"/>
-      <c r="M30" s="31"/>
+      <c r="A30" s="29"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="29"/>
+      <c r="L30" s="29"/>
+      <c r="M30" s="29"/>
       <c r="N30"/>
       <c r="O30"/>
       <c r="P30"/>
@@ -2568,40 +2568,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
       <c r="D1" s="2"/>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="6" t="s">
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="39"/>
+      <c r="W1" s="39"/>
+      <c r="X1" s="39"/>
+      <c r="Y1" s="39"/>
+      <c r="Z1" s="39"/>
+      <c r="AA1" s="39"/>
+      <c r="AB1" s="39"/>
+      <c r="AC1" s="39"/>
       <c r="AM1" t="s">
         <v>0</v>
       </c>
@@ -2640,85 +2640,85 @@
       </c>
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="D2" s="1"/>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="7" t="s">
         <v>35</v>
       </c>
       <c r="J2" s="1"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="9" t="s">
+      <c r="K2" s="9"/>
+      <c r="L2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="N2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="O2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="P2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="Q2" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="R2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="S2" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="T2" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="U2" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="V2" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="W2" s="9" t="s">
+      <c r="W2" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="X2" s="9" t="s">
+      <c r="X2" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="Y2" s="9" t="s">
+      <c r="Y2" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="Z2" s="9" t="s">
+      <c r="Z2" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="AA2" s="9" t="s">
+      <c r="AA2" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="AB2" s="9" t="s">
+      <c r="AB2" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="AC2" s="9" t="s">
+      <c r="AC2" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="AD2" s="9" t="s">
+      <c r="AD2" s="7" t="s">
         <v>54</v>
       </c>
       <c r="AM2" t="s">
@@ -2746,78 +2746,78 @@
         <v>1</v>
       </c>
       <c r="AX2">
-        <f>(SUM(AN2:AW2))/10</f>
+        <f t="shared" ref="AX2:AX19" si="0">(SUM(AN2:AW2))/10</f>
         <v>0.7</v>
       </c>
     </row>
     <row r="3" spans="1:50" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="12">
-        <v>1</v>
-      </c>
-      <c r="C3" s="13">
+      <c r="B3" s="10">
+        <v>1</v>
+      </c>
+      <c r="C3" s="11">
         <f>B3/B6</f>
         <v>0.1</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="F3" s="15">
-        <v>1</v>
-      </c>
-      <c r="G3" s="16" t="s">
+      <c r="D3" s="12"/>
+      <c r="F3" s="13">
+        <v>1</v>
+      </c>
+      <c r="G3" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="19">
-        <v>1</v>
-      </c>
-      <c r="M3" s="19">
-        <v>1</v>
-      </c>
-      <c r="N3" s="19">
-        <v>1</v>
-      </c>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19">
-        <v>1</v>
-      </c>
-      <c r="R3" s="19">
-        <v>1</v>
-      </c>
-      <c r="S3" s="19">
-        <v>1</v>
-      </c>
-      <c r="T3" s="19">
-        <v>1</v>
-      </c>
-      <c r="U3" s="19"/>
-      <c r="V3" s="19"/>
-      <c r="W3" s="19">
-        <v>1</v>
-      </c>
-      <c r="X3" s="19"/>
-      <c r="Y3" s="19"/>
-      <c r="Z3" s="19">
-        <v>1</v>
-      </c>
-      <c r="AA3" s="19">
-        <v>1</v>
-      </c>
-      <c r="AB3" s="19">
-        <v>1</v>
-      </c>
-      <c r="AC3" s="19">
-        <v>1</v>
-      </c>
-      <c r="AD3" s="20">
-        <f t="shared" ref="AD3:AD12" si="0">(SUM(L3:AC3)/18)</f>
+      <c r="I3" s="15"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="17">
+        <v>1</v>
+      </c>
+      <c r="M3" s="17">
+        <v>1</v>
+      </c>
+      <c r="N3" s="17">
+        <v>1</v>
+      </c>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17">
+        <v>1</v>
+      </c>
+      <c r="R3" s="17">
+        <v>1</v>
+      </c>
+      <c r="S3" s="17">
+        <v>1</v>
+      </c>
+      <c r="T3" s="17">
+        <v>1</v>
+      </c>
+      <c r="U3" s="17"/>
+      <c r="V3" s="17"/>
+      <c r="W3" s="17">
+        <v>1</v>
+      </c>
+      <c r="X3" s="17"/>
+      <c r="Y3" s="17"/>
+      <c r="Z3" s="17">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="17">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="17">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="17">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="18">
+        <f t="shared" ref="AD3:AD12" si="1">(SUM(L3:AC3)/18)</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="AM3" t="s">
@@ -2839,89 +2839,89 @@
         <v>1</v>
       </c>
       <c r="AX3">
-        <f>(SUM(AN3:AW3))/10</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:50" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="32">
-        <v>1</v>
-      </c>
-      <c r="C4" s="33">
+      <c r="B4" s="30">
+        <v>1</v>
+      </c>
+      <c r="C4" s="31">
         <f>B4/B6</f>
         <v>0.1</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="F4" s="15">
+      <c r="D4" s="12"/>
+      <c r="F4" s="13">
         <v>2</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="H4" s="34" t="s">
+      <c r="H4" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="I4" s="34"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="35">
-        <v>1</v>
-      </c>
-      <c r="M4" s="35">
-        <v>1</v>
-      </c>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="35">
-        <v>1</v>
-      </c>
-      <c r="R4" s="35">
-        <v>1</v>
-      </c>
-      <c r="S4" s="35">
-        <v>1</v>
-      </c>
-      <c r="T4" s="35">
-        <v>1</v>
-      </c>
-      <c r="U4" s="35">
-        <v>1</v>
-      </c>
-      <c r="V4" s="35">
-        <v>1</v>
-      </c>
-      <c r="W4" s="35">
-        <v>1</v>
-      </c>
-      <c r="X4" s="35">
-        <v>1</v>
-      </c>
-      <c r="Y4" s="35">
-        <v>1</v>
-      </c>
-      <c r="Z4" s="35">
-        <v>1</v>
-      </c>
-      <c r="AA4" s="35">
-        <v>1</v>
-      </c>
-      <c r="AB4" s="35">
-        <v>1</v>
-      </c>
-      <c r="AC4" s="35">
-        <v>1</v>
-      </c>
-      <c r="AD4" s="36">
-        <f t="shared" si="0"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="33">
+        <v>1</v>
+      </c>
+      <c r="M4" s="33">
+        <v>1</v>
+      </c>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="33">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="33">
+        <v>1</v>
+      </c>
+      <c r="R4" s="33">
+        <v>1</v>
+      </c>
+      <c r="S4" s="33">
+        <v>1</v>
+      </c>
+      <c r="T4" s="33">
+        <v>1</v>
+      </c>
+      <c r="U4" s="33">
+        <v>1</v>
+      </c>
+      <c r="V4" s="33">
+        <v>1</v>
+      </c>
+      <c r="W4" s="33">
+        <v>1</v>
+      </c>
+      <c r="X4" s="33">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="33">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="33">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="33">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="33">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="33">
+        <v>1</v>
+      </c>
+      <c r="AD4" s="34">
+        <f t="shared" si="1"/>
         <v>0.88888888888888884</v>
       </c>
-      <c r="AE4" s="18"/>
+      <c r="AE4" s="16"/>
       <c r="AM4" t="s">
         <v>48</v>
       </c>
@@ -2941,83 +2941,83 @@
         <v>1</v>
       </c>
       <c r="AX4">
-        <f>(SUM(AN4:AW4))/10</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:50" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="19">
         <v>8</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="20">
         <f>B5/B6</f>
         <v>0.8</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="F5" s="15">
+      <c r="D5" s="12"/>
+      <c r="F5" s="13">
         <v>3</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="37" t="s">
+      <c r="H5" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="I5" s="37"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="38">
-        <v>1</v>
-      </c>
-      <c r="M5" s="38">
-        <v>1</v>
-      </c>
-      <c r="N5" s="38">
-        <v>1</v>
-      </c>
-      <c r="O5" s="38">
-        <v>1</v>
-      </c>
-      <c r="P5" s="38">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="38"/>
-      <c r="R5" s="38"/>
-      <c r="S5" s="38">
-        <v>1</v>
-      </c>
-      <c r="T5" s="38">
-        <v>1</v>
-      </c>
-      <c r="U5" s="38">
-        <v>1</v>
-      </c>
-      <c r="V5" s="38"/>
-      <c r="W5" s="38">
-        <v>1</v>
-      </c>
-      <c r="X5" s="38">
-        <v>1</v>
-      </c>
-      <c r="Y5" s="38"/>
-      <c r="Z5" s="38"/>
-      <c r="AA5" s="38">
-        <v>1</v>
-      </c>
-      <c r="AB5" s="38">
-        <v>1</v>
-      </c>
-      <c r="AC5" s="38">
-        <v>1</v>
-      </c>
-      <c r="AD5" s="39">
-        <f t="shared" si="0"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="36">
+        <v>1</v>
+      </c>
+      <c r="M5" s="36">
+        <v>1</v>
+      </c>
+      <c r="N5" s="36">
+        <v>1</v>
+      </c>
+      <c r="O5" s="36">
+        <v>1</v>
+      </c>
+      <c r="P5" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="36"/>
+      <c r="R5" s="36"/>
+      <c r="S5" s="36">
+        <v>1</v>
+      </c>
+      <c r="T5" s="36">
+        <v>1</v>
+      </c>
+      <c r="U5" s="36">
+        <v>1</v>
+      </c>
+      <c r="V5" s="36"/>
+      <c r="W5" s="36">
+        <v>1</v>
+      </c>
+      <c r="X5" s="36">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="36"/>
+      <c r="Z5" s="36"/>
+      <c r="AA5" s="36">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="36">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="36">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="37">
+        <f t="shared" si="1"/>
         <v>0.72222222222222221</v>
       </c>
-      <c r="AE5" s="18"/>
+      <c r="AE5" s="16"/>
       <c r="AM5" t="s">
         <v>45</v>
       </c>
@@ -3034,70 +3034,70 @@
         <v>1</v>
       </c>
       <c r="AX5">
-        <f>(SUM(AN5:AW5))/10</f>
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
     </row>
     <row r="6" spans="1:50" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="7">
         <f>SUM(B3:B5)</f>
         <v>10</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="22">
         <f>SUM(C3:C5)</f>
         <v>1</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="F6" s="15">
+      <c r="D6" s="23"/>
+      <c r="F6" s="13">
         <v>4</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="I6" s="37"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="38">
-        <v>1</v>
-      </c>
-      <c r="M6" s="38">
-        <v>1</v>
-      </c>
-      <c r="N6" s="38"/>
-      <c r="O6" s="38"/>
-      <c r="P6" s="38">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="38"/>
-      <c r="R6" s="38"/>
-      <c r="S6" s="38">
-        <v>1</v>
-      </c>
-      <c r="T6" s="38"/>
-      <c r="U6" s="38"/>
-      <c r="V6" s="38"/>
-      <c r="W6" s="38"/>
-      <c r="X6" s="38">
-        <v>1</v>
-      </c>
-      <c r="Y6" s="38"/>
-      <c r="Z6" s="38"/>
-      <c r="AA6" s="38"/>
-      <c r="AB6" s="38"/>
-      <c r="AC6" s="38">
-        <v>1</v>
-      </c>
-      <c r="AD6" s="39">
-        <f t="shared" si="0"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="36">
+        <v>1</v>
+      </c>
+      <c r="M6" s="36">
+        <v>1</v>
+      </c>
+      <c r="N6" s="36"/>
+      <c r="O6" s="36"/>
+      <c r="P6" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="36"/>
+      <c r="R6" s="36"/>
+      <c r="S6" s="36">
+        <v>1</v>
+      </c>
+      <c r="T6" s="36"/>
+      <c r="U6" s="36"/>
+      <c r="V6" s="36"/>
+      <c r="W6" s="36"/>
+      <c r="X6" s="36">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="36"/>
+      <c r="Z6" s="36"/>
+      <c r="AA6" s="36"/>
+      <c r="AB6" s="36"/>
+      <c r="AC6" s="36">
+        <v>1</v>
+      </c>
+      <c r="AD6" s="37">
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="AE6" s="18"/>
+      <c r="AE6" s="16"/>
       <c r="AM6" t="s">
         <v>43</v>
       </c>
@@ -3126,74 +3126,74 @@
         <v>1</v>
       </c>
       <c r="AX6">
-        <f>(SUM(AN6:AW6))/10</f>
+        <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
     </row>
     <row r="7" spans="1:50" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="F7" s="15">
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="F7" s="13">
         <v>5</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="H7" s="37" t="s">
+      <c r="H7" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="I7" s="37"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="38">
-        <v>1</v>
-      </c>
-      <c r="M7" s="38">
-        <v>1</v>
-      </c>
-      <c r="N7" s="38">
-        <v>1</v>
-      </c>
-      <c r="O7" s="38">
-        <v>1</v>
-      </c>
-      <c r="P7" s="38">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="38"/>
-      <c r="R7" s="38"/>
-      <c r="S7" s="38">
-        <v>1</v>
-      </c>
-      <c r="T7" s="38">
-        <v>1</v>
-      </c>
-      <c r="U7" s="38">
-        <v>1</v>
-      </c>
-      <c r="V7" s="38">
-        <v>1</v>
-      </c>
-      <c r="W7" s="38">
-        <v>1</v>
-      </c>
-      <c r="X7" s="38"/>
-      <c r="Y7" s="38">
-        <v>1</v>
-      </c>
-      <c r="Z7" s="38"/>
-      <c r="AA7" s="38"/>
-      <c r="AB7" s="38">
-        <v>1</v>
-      </c>
-      <c r="AC7" s="38"/>
-      <c r="AD7" s="39">
-        <f t="shared" si="0"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="36">
+        <v>1</v>
+      </c>
+      <c r="M7" s="36">
+        <v>1</v>
+      </c>
+      <c r="N7" s="36">
+        <v>1</v>
+      </c>
+      <c r="O7" s="36">
+        <v>1</v>
+      </c>
+      <c r="P7" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="36"/>
+      <c r="R7" s="36"/>
+      <c r="S7" s="36">
+        <v>1</v>
+      </c>
+      <c r="T7" s="36">
+        <v>1</v>
+      </c>
+      <c r="U7" s="36">
+        <v>1</v>
+      </c>
+      <c r="V7" s="36">
+        <v>1</v>
+      </c>
+      <c r="W7" s="36">
+        <v>1</v>
+      </c>
+      <c r="X7" s="36"/>
+      <c r="Y7" s="36">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="36"/>
+      <c r="AA7" s="36"/>
+      <c r="AB7" s="36">
+        <v>1</v>
+      </c>
+      <c r="AC7" s="36"/>
+      <c r="AD7" s="37">
+        <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="AE7" s="18"/>
+      <c r="AE7" s="16"/>
       <c r="AM7" t="s">
         <v>38</v>
       </c>
@@ -3210,72 +3210,72 @@
         <v>1</v>
       </c>
       <c r="AX7">
-        <f>(SUM(AN7:AW7))/10</f>
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
     </row>
     <row r="8" spans="1:50" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="F8" s="15">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="F8" s="13">
         <v>6</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="H8" s="37" t="s">
+      <c r="H8" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="I8" s="37"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="38">
-        <v>1</v>
-      </c>
-      <c r="M8" s="38">
-        <v>1</v>
-      </c>
-      <c r="N8" s="38"/>
-      <c r="O8" s="38"/>
-      <c r="P8" s="38">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="38"/>
-      <c r="R8" s="38">
-        <v>1</v>
-      </c>
-      <c r="S8" s="38">
-        <v>1</v>
-      </c>
-      <c r="T8" s="38">
-        <v>1</v>
-      </c>
-      <c r="U8" s="38">
-        <v>1</v>
-      </c>
-      <c r="V8" s="38"/>
-      <c r="W8" s="38"/>
-      <c r="X8" s="38">
-        <v>1</v>
-      </c>
-      <c r="Y8" s="38">
-        <v>1</v>
-      </c>
-      <c r="Z8" s="38">
-        <v>1</v>
-      </c>
-      <c r="AA8" s="38"/>
-      <c r="AB8" s="38"/>
-      <c r="AC8" s="38">
-        <v>1</v>
-      </c>
-      <c r="AD8" s="39">
-        <f t="shared" si="0"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="36">
+        <v>1</v>
+      </c>
+      <c r="M8" s="36">
+        <v>1</v>
+      </c>
+      <c r="N8" s="36"/>
+      <c r="O8" s="36"/>
+      <c r="P8" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="36"/>
+      <c r="R8" s="36">
+        <v>1</v>
+      </c>
+      <c r="S8" s="36">
+        <v>1</v>
+      </c>
+      <c r="T8" s="36">
+        <v>1</v>
+      </c>
+      <c r="U8" s="36">
+        <v>1</v>
+      </c>
+      <c r="V8" s="36"/>
+      <c r="W8" s="36"/>
+      <c r="X8" s="36">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="36">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="36">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="36"/>
+      <c r="AB8" s="36"/>
+      <c r="AC8" s="36">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="37">
+        <f t="shared" si="1"/>
         <v>0.61111111111111116</v>
       </c>
-      <c r="AE8" s="18"/>
+      <c r="AE8" s="16"/>
       <c r="AM8" t="s">
         <v>36</v>
       </c>
@@ -3307,74 +3307,74 @@
         <v>1</v>
       </c>
       <c r="AX8">
-        <f>(SUM(AN8:AW8))/10</f>
+        <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
     </row>
     <row r="9" spans="1:50" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="F9" s="15">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="F9" s="13">
         <v>7</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="H9" s="37" t="s">
+      <c r="H9" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="37"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="38">
-        <v>1</v>
-      </c>
-      <c r="M9" s="38">
-        <v>1</v>
-      </c>
-      <c r="N9" s="38">
-        <v>1</v>
-      </c>
-      <c r="O9" s="38">
-        <v>1</v>
-      </c>
-      <c r="P9" s="38">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="38"/>
-      <c r="R9" s="38"/>
-      <c r="S9" s="38">
-        <v>1</v>
-      </c>
-      <c r="T9" s="38"/>
-      <c r="U9" s="38"/>
-      <c r="V9" s="38">
-        <v>1</v>
-      </c>
-      <c r="W9" s="38">
-        <v>1</v>
-      </c>
-      <c r="X9" s="38">
-        <v>1</v>
-      </c>
-      <c r="Y9" s="38">
-        <v>1</v>
-      </c>
-      <c r="Z9" s="38">
-        <v>1</v>
-      </c>
-      <c r="AA9" s="38"/>
-      <c r="AB9" s="38">
-        <v>1</v>
-      </c>
-      <c r="AC9" s="38"/>
-      <c r="AD9" s="39">
-        <f t="shared" si="0"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="36">
+        <v>1</v>
+      </c>
+      <c r="M9" s="36">
+        <v>1</v>
+      </c>
+      <c r="N9" s="36">
+        <v>1</v>
+      </c>
+      <c r="O9" s="36">
+        <v>1</v>
+      </c>
+      <c r="P9" s="36">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="36"/>
+      <c r="R9" s="36"/>
+      <c r="S9" s="36">
+        <v>1</v>
+      </c>
+      <c r="T9" s="36"/>
+      <c r="U9" s="36"/>
+      <c r="V9" s="36">
+        <v>1</v>
+      </c>
+      <c r="W9" s="36">
+        <v>1</v>
+      </c>
+      <c r="X9" s="36">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="36">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="36">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="36"/>
+      <c r="AB9" s="36">
+        <v>1</v>
+      </c>
+      <c r="AC9" s="36"/>
+      <c r="AD9" s="37">
+        <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="AE9" s="18"/>
+      <c r="AE9" s="16"/>
       <c r="AM9" t="s">
         <v>44</v>
       </c>
@@ -3400,70 +3400,70 @@
         <v>1</v>
       </c>
       <c r="AX9">
-        <f>(SUM(AN9:AW9))/10</f>
+        <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
     </row>
     <row r="10" spans="1:50" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="18"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="F10" s="15">
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="F10" s="13">
         <v>8</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="H10" s="37" t="s">
+      <c r="H10" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="I10" s="37"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="38">
-        <v>1</v>
-      </c>
-      <c r="M10" s="38"/>
-      <c r="N10" s="38"/>
-      <c r="O10" s="38"/>
-      <c r="P10" s="38"/>
-      <c r="Q10" s="38">
-        <v>1</v>
-      </c>
-      <c r="R10" s="38"/>
-      <c r="S10" s="38">
-        <v>1</v>
-      </c>
-      <c r="T10" s="38">
-        <v>1</v>
-      </c>
-      <c r="U10" s="38"/>
-      <c r="V10" s="38">
-        <v>1</v>
-      </c>
-      <c r="W10" s="38">
-        <v>1</v>
-      </c>
-      <c r="X10" s="38"/>
-      <c r="Y10" s="38">
-        <v>1</v>
-      </c>
-      <c r="Z10" s="38">
-        <v>1</v>
-      </c>
-      <c r="AA10" s="38">
-        <v>1</v>
-      </c>
-      <c r="AB10" s="38">
-        <v>1</v>
-      </c>
-      <c r="AC10" s="38"/>
-      <c r="AD10" s="39">
-        <f t="shared" si="0"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="36">
+        <v>1</v>
+      </c>
+      <c r="M10" s="36"/>
+      <c r="N10" s="36"/>
+      <c r="O10" s="36"/>
+      <c r="P10" s="36"/>
+      <c r="Q10" s="36">
+        <v>1</v>
+      </c>
+      <c r="R10" s="36"/>
+      <c r="S10" s="36">
+        <v>1</v>
+      </c>
+      <c r="T10" s="36">
+        <v>1</v>
+      </c>
+      <c r="U10" s="36"/>
+      <c r="V10" s="36">
+        <v>1</v>
+      </c>
+      <c r="W10" s="36">
+        <v>1</v>
+      </c>
+      <c r="X10" s="36"/>
+      <c r="Y10" s="36">
+        <v>1</v>
+      </c>
+      <c r="Z10" s="36">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="36">
+        <v>1</v>
+      </c>
+      <c r="AB10" s="36">
+        <v>1</v>
+      </c>
+      <c r="AC10" s="36"/>
+      <c r="AD10" s="37">
+        <f t="shared" si="1"/>
         <v>0.55555555555555558</v>
       </c>
-      <c r="AE10" s="18"/>
+      <c r="AE10" s="16"/>
       <c r="AM10" t="s">
         <v>49</v>
       </c>
@@ -3483,60 +3483,60 @@
         <v>1</v>
       </c>
       <c r="AX10">
-        <f>(SUM(AN10:AW10))/10</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:50" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="F11" s="15">
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="F11" s="13">
         <v>9</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="H11" s="37" t="s">
+      <c r="H11" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="I11" s="37"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="38">
-        <v>1</v>
-      </c>
-      <c r="M11" s="38"/>
-      <c r="N11" s="38"/>
-      <c r="O11" s="38"/>
-      <c r="P11" s="38"/>
-      <c r="Q11" s="38"/>
-      <c r="R11" s="38">
-        <v>1</v>
-      </c>
-      <c r="S11" s="38"/>
-      <c r="T11" s="38">
-        <v>1</v>
-      </c>
-      <c r="U11" s="38"/>
-      <c r="V11" s="38"/>
-      <c r="W11" s="38"/>
-      <c r="X11" s="38"/>
-      <c r="Y11" s="38"/>
-      <c r="Z11" s="38">
-        <v>1</v>
-      </c>
-      <c r="AA11" s="38">
-        <v>1</v>
-      </c>
-      <c r="AB11" s="38"/>
-      <c r="AC11" s="38"/>
-      <c r="AD11" s="39">
-        <f t="shared" si="0"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="36">
+        <v>1</v>
+      </c>
+      <c r="M11" s="36"/>
+      <c r="N11" s="36"/>
+      <c r="O11" s="36"/>
+      <c r="P11" s="36"/>
+      <c r="Q11" s="36"/>
+      <c r="R11" s="36">
+        <v>1</v>
+      </c>
+      <c r="S11" s="36"/>
+      <c r="T11" s="36">
+        <v>1</v>
+      </c>
+      <c r="U11" s="36"/>
+      <c r="V11" s="36"/>
+      <c r="W11" s="36"/>
+      <c r="X11" s="36"/>
+      <c r="Y11" s="36"/>
+      <c r="Z11" s="36">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="36">
+        <v>1</v>
+      </c>
+      <c r="AB11" s="36"/>
+      <c r="AC11" s="36"/>
+      <c r="AD11" s="37">
+        <f t="shared" si="1"/>
         <v>0.27777777777777779</v>
       </c>
-      <c r="AE11" s="18"/>
+      <c r="AE11" s="16"/>
       <c r="AM11" t="s">
         <v>47</v>
       </c>
@@ -3559,54 +3559,54 @@
         <v>1</v>
       </c>
       <c r="AX11">
-        <f>(SUM(AN11:AW11))/10</f>
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
     <row r="12" spans="1:50" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="F12" s="15">
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="F12" s="13">
         <v>10</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="H12" s="37" t="s">
+      <c r="H12" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="I12" s="37"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="38"/>
-      <c r="N12" s="38"/>
-      <c r="O12" s="38">
-        <v>1</v>
-      </c>
-      <c r="P12" s="38"/>
-      <c r="Q12" s="38"/>
-      <c r="R12" s="38"/>
-      <c r="S12" s="38"/>
-      <c r="T12" s="38"/>
-      <c r="U12" s="38"/>
-      <c r="V12" s="38"/>
-      <c r="W12" s="38"/>
-      <c r="X12" s="38"/>
-      <c r="Y12" s="38"/>
-      <c r="Z12" s="38"/>
-      <c r="AA12" s="38"/>
-      <c r="AB12" s="38"/>
-      <c r="AC12" s="38">
-        <v>1</v>
-      </c>
-      <c r="AD12" s="39">
-        <f t="shared" si="0"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="36">
+        <v>1</v>
+      </c>
+      <c r="P12" s="36"/>
+      <c r="Q12" s="36"/>
+      <c r="R12" s="36"/>
+      <c r="S12" s="36"/>
+      <c r="T12" s="36"/>
+      <c r="U12" s="36"/>
+      <c r="V12" s="36"/>
+      <c r="W12" s="36"/>
+      <c r="X12" s="36"/>
+      <c r="Y12" s="36"/>
+      <c r="Z12" s="36"/>
+      <c r="AA12" s="36"/>
+      <c r="AB12" s="36"/>
+      <c r="AC12" s="36">
+        <v>1</v>
+      </c>
+      <c r="AD12" s="37">
+        <f t="shared" si="1"/>
         <v>0.1111111111111111</v>
       </c>
-      <c r="AE12" s="18"/>
+      <c r="AE12" s="16"/>
       <c r="AM12" t="s">
         <v>42</v>
       </c>
@@ -3623,99 +3623,99 @@
         <v>1</v>
       </c>
       <c r="AX12">
-        <f>(SUM(AN12:AW12))/10</f>
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
     </row>
     <row r="13" spans="1:50" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="27" t="s">
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="L13" s="28">
-        <f t="shared" ref="L13:AC13" si="1">(SUM(L3:L12))/10</f>
+      <c r="L13" s="26">
+        <f t="shared" ref="L13:AC13" si="2">(SUM(L3:L12))/10</f>
         <v>0.9</v>
       </c>
-      <c r="M13" s="28">
-        <f t="shared" si="1"/>
+      <c r="M13" s="26">
+        <f t="shared" si="2"/>
         <v>0.7</v>
       </c>
-      <c r="N13" s="28">
-        <f t="shared" si="1"/>
+      <c r="N13" s="26">
+        <f t="shared" si="2"/>
         <v>0.4</v>
       </c>
-      <c r="O13" s="28">
-        <f t="shared" si="1"/>
+      <c r="O13" s="26">
+        <f t="shared" si="2"/>
         <v>0.4</v>
       </c>
-      <c r="P13" s="28">
-        <f t="shared" si="1"/>
+      <c r="P13" s="26">
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
-      <c r="Q13" s="28">
-        <f t="shared" si="1"/>
+      <c r="Q13" s="26">
+        <f t="shared" si="2"/>
         <v>0.3</v>
       </c>
-      <c r="R13" s="28">
-        <f t="shared" si="1"/>
+      <c r="R13" s="26">
+        <f t="shared" si="2"/>
         <v>0.4</v>
       </c>
-      <c r="S13" s="28">
-        <f t="shared" si="1"/>
+      <c r="S13" s="26">
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
-      <c r="T13" s="28">
-        <f t="shared" si="1"/>
+      <c r="T13" s="26">
+        <f t="shared" si="2"/>
         <v>0.7</v>
       </c>
-      <c r="U13" s="28">
-        <f t="shared" si="1"/>
+      <c r="U13" s="26">
+        <f t="shared" si="2"/>
         <v>0.4</v>
       </c>
-      <c r="V13" s="28">
-        <f t="shared" si="1"/>
+      <c r="V13" s="26">
+        <f t="shared" si="2"/>
         <v>0.4</v>
       </c>
-      <c r="W13" s="28">
-        <f t="shared" si="1"/>
+      <c r="W13" s="26">
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
-      <c r="X13" s="28">
-        <f t="shared" si="1"/>
+      <c r="X13" s="26">
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="Y13" s="28">
-        <f t="shared" si="1"/>
+      <c r="Y13" s="26">
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="Z13" s="28">
-        <f t="shared" si="1"/>
+      <c r="Z13" s="26">
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
-      <c r="AA13" s="28">
-        <f t="shared" si="1"/>
+      <c r="AA13" s="26">
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="AB13" s="28">
-        <f t="shared" si="1"/>
+      <c r="AB13" s="26">
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
-      <c r="AC13" s="28">
-        <f t="shared" si="1"/>
+      <c r="AC13" s="26">
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
-      <c r="AD13" s="9" t="s">
+      <c r="AD13" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="AE13" s="18"/>
+      <c r="AE13" s="16"/>
       <c r="AM13" t="s">
         <v>50</v>
       </c>
@@ -3738,49 +3738,49 @@
         <v>1</v>
       </c>
       <c r="AX13">
-        <f>(SUM(AN13:AW13))/10</f>
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
     <row r="14" spans="1:50" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="29" t="s">
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="L14" s="30">
+      <c r="L14" s="28">
         <f>AVERAGE(L13:AC13)</f>
         <v>0.55000000000000004</v>
       </c>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
-      <c r="V14" s="18"/>
-      <c r="W14" s="18"/>
-      <c r="X14" s="18"/>
-      <c r="Y14" s="18"/>
-      <c r="Z14" s="18"/>
-      <c r="AA14" s="18"/>
-      <c r="AB14" s="18"/>
-      <c r="AC14" s="18"/>
-      <c r="AD14" s="28">
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="16"/>
+      <c r="T14" s="16"/>
+      <c r="U14" s="16"/>
+      <c r="V14" s="16"/>
+      <c r="W14" s="16"/>
+      <c r="X14" s="16"/>
+      <c r="Y14" s="16"/>
+      <c r="Z14" s="16"/>
+      <c r="AA14" s="16"/>
+      <c r="AB14" s="16"/>
+      <c r="AC14" s="16"/>
+      <c r="AD14" s="26">
         <f>AVERAGE(AD3:AD12)</f>
         <v>0.54999999999999993</v>
       </c>
-      <c r="AE14" s="18"/>
+      <c r="AE14" s="16"/>
       <c r="AM14" t="s">
         <v>46</v>
       </c>
@@ -3797,7 +3797,7 @@
         <v>1</v>
       </c>
       <c r="AX14">
-        <f>(SUM(AN14:AW14))/10</f>
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
     </row>
@@ -3824,7 +3824,7 @@
         <v>1</v>
       </c>
       <c r="AX15">
-        <f>(SUM(AN15:AW15))/10</f>
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -3845,7 +3845,7 @@
         <v>1</v>
       </c>
       <c r="AX16">
-        <f>(SUM(AN16:AW16))/10</f>
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
     </row>
@@ -3872,7 +3872,7 @@
         <v>1</v>
       </c>
       <c r="AX17">
-        <f>(SUM(AN17:AW17))/10</f>
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -3899,7 +3899,7 @@
         <v>1</v>
       </c>
       <c r="AX18">
-        <f>(SUM(AN18:AW18))/10</f>
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -3917,7 +3917,7 @@
         <v>1</v>
       </c>
       <c r="AX19">
-        <f>(SUM(AN19:AW19))/10</f>
+        <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
upload variables with values
</commit_message>
<xml_diff>
--- a/localExperiments/hazardIdentification/hazardIdentification.xlsx
+++ b/localExperiments/hazardIdentification/hazardIdentification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattsears/code/eyetracker/localExperiments/hazardIdentification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96094CB-E6DE-444E-BE6D-96A3CB134A0C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28047DEF-6C4A-B04C-A044-3919FF5D6ADC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19000" xr2:uid="{3006803E-C1FE-6049-930A-55B4D31C99D5}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'A Dylan Data'!$AM$1:$AX$19</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">hazardIdentification!$A$1:$W$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">hazardIdentification!$A$1:$V$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="90">
   <si>
     <t>Name</t>
   </si>
@@ -55,63 +55,6 @@
     <t>C HR Index</t>
   </si>
   <si>
-    <t>aaron</t>
-  </si>
-  <si>
-    <t>aby</t>
-  </si>
-  <si>
-    <t>brian</t>
-  </si>
-  <si>
-    <t>david</t>
-  </si>
-  <si>
-    <t>doug</t>
-  </si>
-  <si>
-    <t>gabe</t>
-  </si>
-  <si>
-    <t>james</t>
-  </si>
-  <si>
-    <t>jessica</t>
-  </si>
-  <si>
-    <t>joe</t>
-  </si>
-  <si>
-    <t>katie</t>
-  </si>
-  <si>
-    <t>kyle</t>
-  </si>
-  <si>
-    <t>nathan </t>
-  </si>
-  <si>
-    <t>sara</t>
-  </si>
-  <si>
-    <t>sid</t>
-  </si>
-  <si>
-    <t>sravan</t>
-  </si>
-  <si>
-    <t>ulises</t>
-  </si>
-  <si>
-    <t>wael</t>
-  </si>
-  <si>
-    <t>Partiicpant #</t>
-  </si>
-  <si>
-    <t>guillermo</t>
-  </si>
-  <si>
     <t>viewingDuration</t>
   </si>
   <si>
@@ -311,6 +254,60 @@
   </si>
   <si>
     <t>HRPS</t>
+  </si>
+  <si>
+    <t>001_wael</t>
+  </si>
+  <si>
+    <t>002_ulises</t>
+  </si>
+  <si>
+    <t>003_sravan</t>
+  </si>
+  <si>
+    <t>004_sid</t>
+  </si>
+  <si>
+    <t>005_sara</t>
+  </si>
+  <si>
+    <t>006_nathan </t>
+  </si>
+  <si>
+    <t>007_kyle</t>
+  </si>
+  <si>
+    <t>008_katie</t>
+  </si>
+  <si>
+    <t>009_joe</t>
+  </si>
+  <si>
+    <t>010_jessica</t>
+  </si>
+  <si>
+    <t>011_james</t>
+  </si>
+  <si>
+    <t>012_guillermo</t>
+  </si>
+  <si>
+    <t>013_gabe</t>
+  </si>
+  <si>
+    <t>014_doug</t>
+  </si>
+  <si>
+    <t>015_david</t>
+  </si>
+  <si>
+    <t>016_brian</t>
+  </si>
+  <si>
+    <t>017_aby</t>
+  </si>
+  <si>
+    <t>018_aaron</t>
   </si>
 </sst>
 </file>
@@ -821,192 +818,185 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E7DCC3D-D30E-6243-939A-246A0296DDAF}">
-  <dimension ref="A1:W32"/>
+  <dimension ref="A1:V32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S30" sqref="S30"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="13" width="5.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="10.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="12" width="5.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>89</v>
+        <v>53</v>
       </c>
       <c r="N1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>72</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="B2">
+        <v>0.68707483000000003</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0</v>
+      </c>
+      <c r="M2" s="3">
+        <f t="shared" ref="M2:M19" si="0">C2</f>
+        <v>1</v>
+      </c>
+      <c r="N2" s="3">
+        <f t="shared" ref="N2:N19" si="1">M2</f>
+        <v>1</v>
+      </c>
+      <c r="O2" s="3">
+        <f t="shared" ref="O2:O19" si="2">D2</f>
+        <v>1</v>
+      </c>
+      <c r="P2" s="3">
+        <f t="shared" ref="P2:P19" si="3">O2</f>
+        <v>1</v>
+      </c>
+      <c r="Q2" s="3">
+        <f t="shared" ref="Q2:Q19" si="4">SUM(E2:L2)</f>
+        <v>1</v>
+      </c>
+      <c r="R2" s="3">
+        <f t="shared" ref="R2:R19" si="5">Q2/8</f>
+        <v>0.125</v>
+      </c>
+      <c r="S2" s="3">
+        <f t="shared" ref="S2:S19" si="6">M2+O2+Q2</f>
+        <v>3</v>
+      </c>
+      <c r="T2" s="3">
+        <f>S2/'A Dylan Data'!$B$6</f>
+        <v>0.3</v>
+      </c>
+      <c r="U2" s="3">
+        <v>87607</v>
+      </c>
+      <c r="V2" s="3">
+        <f t="shared" ref="V2:V19" si="7">S2/U2*1000</f>
+        <v>3.4243838962639973E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>73</v>
       </c>
-      <c r="P1" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2">
-        <v>0.68707483000000003</v>
-      </c>
-      <c r="D2" s="3">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3">
-        <v>1</v>
-      </c>
-      <c r="F2" s="3">
-        <v>0</v>
-      </c>
-      <c r="G2" s="3">
-        <v>0</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0</v>
-      </c>
-      <c r="I2" s="3">
-        <v>0</v>
-      </c>
-      <c r="J2" s="3">
-        <v>0</v>
-      </c>
-      <c r="K2" s="3">
-        <v>1</v>
-      </c>
-      <c r="L2" s="3">
-        <v>0</v>
-      </c>
-      <c r="M2" s="3">
-        <v>0</v>
-      </c>
-      <c r="N2" s="3">
-        <f t="shared" ref="N2:N19" si="0">D2</f>
-        <v>1</v>
-      </c>
-      <c r="O2" s="3">
-        <f t="shared" ref="O2:O19" si="1">N2</f>
-        <v>1</v>
-      </c>
-      <c r="P2" s="3">
-        <f t="shared" ref="P2:P19" si="2">E2</f>
-        <v>1</v>
-      </c>
-      <c r="Q2" s="3">
-        <f t="shared" ref="Q2:Q19" si="3">P2</f>
-        <v>1</v>
-      </c>
-      <c r="R2" s="3">
-        <f t="shared" ref="R2:R19" si="4">SUM(F2:M2)</f>
-        <v>1</v>
-      </c>
-      <c r="S2" s="3">
-        <f t="shared" ref="S2:S19" si="5">R2/8</f>
-        <v>0.125</v>
-      </c>
-      <c r="T2" s="3">
-        <f t="shared" ref="T2:T19" si="6">N2+P2+R2</f>
-        <v>3</v>
-      </c>
-      <c r="U2" s="3">
-        <f>T2/'A Dylan Data'!$B$6</f>
-        <v>0.3</v>
-      </c>
-      <c r="V2" s="3">
-        <v>87607</v>
-      </c>
-      <c r="W2" s="3">
-        <f t="shared" ref="W2:W19" si="7">T2/V2*1000</f>
-        <v>3.4243838962639973E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3">
+      <c r="B3">
         <v>0.695238095</v>
       </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
       <c r="D3" s="3">
         <v>1</v>
       </c>
@@ -1014,81 +1004,78 @@
         <v>1</v>
       </c>
       <c r="F3" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" s="3">
         <v>1</v>
       </c>
       <c r="K3" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3" s="3">
         <v>0</v>
       </c>
       <c r="M3" s="3">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="N3" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="O3" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P3" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="Q3" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="R3" s="3">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="S3" s="3">
+      <c r="R3" s="3">
         <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
-      <c r="T3" s="3">
+      <c r="S3" s="3">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
+      <c r="T3" s="3">
+        <f>S3/'A Dylan Data'!$B$6</f>
+        <v>0.6</v>
+      </c>
       <c r="U3" s="3">
-        <f>T3/'A Dylan Data'!$B$6</f>
-        <v>0.6</v>
+        <v>129725</v>
       </c>
       <c r="V3" s="3">
-        <v>129725</v>
-      </c>
-      <c r="W3" s="3">
         <f t="shared" si="7"/>
         <v>4.6251686259394874E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4">
         <v>0.69841269800000005</v>
       </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
       <c r="D4" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="3">
         <v>1</v>
@@ -1106,7 +1093,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" s="3">
         <v>0</v>
@@ -1115,138 +1102,132 @@
         <v>0</v>
       </c>
       <c r="M4" s="3">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O4" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="P4" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="Q4" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="R4" s="3">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="S4" s="3">
+      <c r="R4" s="3">
         <f t="shared" si="5"/>
         <v>0.625</v>
       </c>
-      <c r="T4" s="3">
+      <c r="S4" s="3">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
+      <c r="T4" s="3">
+        <f>S4/'A Dylan Data'!$B$6</f>
+        <v>0.6</v>
+      </c>
       <c r="U4" s="3">
-        <f>T4/'A Dylan Data'!$B$6</f>
-        <v>0.6</v>
+        <v>85085</v>
       </c>
       <c r="V4" s="3">
-        <v>85085</v>
-      </c>
-      <c r="W4" s="3">
         <f t="shared" si="7"/>
         <v>7.05177175765411E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5">
         <v>0.75438596499999999</v>
       </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
       <c r="D5" s="3">
         <v>0</v>
       </c>
       <c r="E5" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5" s="3">
         <v>0</v>
       </c>
       <c r="L5" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5" s="3">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="N5" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O5" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P5" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q5" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="R5" s="3">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="S5" s="3">
+      <c r="R5" s="3">
         <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
-      <c r="T5" s="3">
+      <c r="S5" s="3">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
+      <c r="T5" s="3">
+        <f>S5/'A Dylan Data'!$B$6</f>
+        <v>0.4</v>
+      </c>
       <c r="U5" s="3">
-        <f>T5/'A Dylan Data'!$B$6</f>
-        <v>0.4</v>
+        <v>72289</v>
       </c>
       <c r="V5" s="3">
-        <v>72289</v>
-      </c>
-      <c r="W5" s="3">
         <f t="shared" si="7"/>
         <v>5.5333453222481982E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6">
         <v>0.69142857099999999</v>
       </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
       <c r="D6" s="3">
         <v>1</v>
       </c>
@@ -1257,13 +1238,13 @@
         <v>1</v>
       </c>
       <c r="G6" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" s="3">
         <v>0</v>
@@ -1272,146 +1253,140 @@
         <v>0</v>
       </c>
       <c r="L6" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6" s="3">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="O6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P6" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="Q6" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="R6" s="3">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="S6" s="3">
+      <c r="R6" s="3">
         <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
-      <c r="T6" s="3">
+      <c r="S6" s="3">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
+      <c r="T6" s="3">
+        <f>S6/'A Dylan Data'!$B$6</f>
+        <v>0.6</v>
+      </c>
       <c r="U6" s="3">
-        <f>T6/'A Dylan Data'!$B$6</f>
-        <v>0.6</v>
+        <v>97165</v>
       </c>
       <c r="V6" s="3">
-        <v>97165</v>
-      </c>
-      <c r="W6" s="3">
         <f t="shared" si="7"/>
         <v>6.1750630371018377E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7">
         <v>0.728971963</v>
       </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
       <c r="D7" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="3">
         <v>0</v>
       </c>
       <c r="G7" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" s="3">
         <v>1</v>
       </c>
       <c r="K7" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7" s="3">
         <v>0</v>
       </c>
       <c r="M7" s="3">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N7" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O7" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="P7" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="Q7" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="R7" s="3">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="S7" s="3">
+      <c r="R7" s="3">
         <f t="shared" si="5"/>
         <v>0.375</v>
       </c>
-      <c r="T7" s="3">
+      <c r="S7" s="3">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
+      <c r="T7" s="3">
+        <f>S7/'A Dylan Data'!$B$6</f>
+        <v>0.4</v>
+      </c>
       <c r="U7" s="3">
-        <f>T7/'A Dylan Data'!$B$6</f>
-        <v>0.4</v>
+        <v>60706</v>
       </c>
       <c r="V7" s="3">
-        <v>60706</v>
-      </c>
-      <c r="W7" s="3">
         <f t="shared" si="7"/>
         <v>6.5891345171811694E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8">
         <v>0.76666666699999997</v>
       </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
       <c r="D8" s="3">
         <v>1</v>
       </c>
       <c r="E8" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="3">
         <v>0</v>
@@ -1420,7 +1395,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="3">
         <v>1</v>
@@ -1432,66 +1407,63 @@
         <v>1</v>
       </c>
       <c r="L8" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8" s="3">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="N8" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="O8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P8" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="Q8" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="R8" s="3">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="S8" s="3">
+      <c r="R8" s="3">
         <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
-      <c r="T8" s="3">
+      <c r="S8" s="3">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
+      <c r="T8" s="3">
+        <f>S8/'A Dylan Data'!$B$6</f>
+        <v>0.6</v>
+      </c>
       <c r="U8" s="3">
-        <f>T8/'A Dylan Data'!$B$6</f>
-        <v>0.6</v>
+        <v>97978</v>
       </c>
       <c r="V8" s="3">
-        <v>97978</v>
-      </c>
-      <c r="W8" s="3">
         <f t="shared" si="7"/>
         <v>6.1238237155279762E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9">
         <v>0.78666666699999999</v>
       </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
       <c r="D9" s="3">
         <v>1</v>
       </c>
       <c r="E9" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="3">
         <v>0</v>
@@ -1500,73 +1472,70 @@
         <v>0</v>
       </c>
       <c r="H9" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" s="3">
         <v>0</v>
       </c>
       <c r="K9" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9" s="3">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="N9" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="O9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P9" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="Q9" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="R9" s="3">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="S9" s="3">
+      <c r="R9" s="3">
         <f t="shared" si="5"/>
         <v>0.25</v>
       </c>
-      <c r="T9" s="3">
+      <c r="S9" s="3">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
+      <c r="T9" s="3">
+        <f>S9/'A Dylan Data'!$B$6</f>
+        <v>0.4</v>
+      </c>
       <c r="U9" s="3">
-        <f>T9/'A Dylan Data'!$B$6</f>
-        <v>0.4</v>
+        <v>34269</v>
       </c>
       <c r="V9" s="3">
-        <v>34269</v>
-      </c>
-      <c r="W9" s="3">
         <f t="shared" si="7"/>
         <v>0.11672356940675246</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10">
         <v>0.73983739800000003</v>
       </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
       <c r="D10" s="3">
         <v>1</v>
       </c>
@@ -1574,90 +1543,87 @@
         <v>1</v>
       </c>
       <c r="F10" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="3">
         <v>1</v>
       </c>
       <c r="K10" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L10" s="3">
         <v>0</v>
       </c>
       <c r="M10" s="3">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="N10" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="O10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P10" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="Q10" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="R10" s="3">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="S10" s="3">
+      <c r="R10" s="3">
         <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
-      <c r="T10" s="3">
+      <c r="S10" s="3">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
+      <c r="T10" s="3">
+        <f>S10/'A Dylan Data'!$B$6</f>
+        <v>0.6</v>
+      </c>
       <c r="U10" s="3">
-        <f>T10/'A Dylan Data'!$B$6</f>
-        <v>0.6</v>
+        <v>52640</v>
       </c>
       <c r="V10" s="3">
-        <v>52640</v>
-      </c>
-      <c r="W10" s="3">
         <f t="shared" si="7"/>
         <v>0.11398176291793312</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11">
         <v>0.73684210500000002</v>
       </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
       <c r="D11" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="3">
         <v>0</v>
       </c>
       <c r="G11" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="3">
         <v>1</v>
@@ -1669,64 +1635,61 @@
         <v>1</v>
       </c>
       <c r="K11" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11" s="3">
         <v>0</v>
       </c>
       <c r="M11" s="3">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N11" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O11" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="P11" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="Q11" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="R11" s="3">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="S11" s="3">
+      <c r="R11" s="3">
         <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
-      <c r="T11" s="3">
+      <c r="S11" s="3">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
+      <c r="T11" s="3">
+        <f>S11/'A Dylan Data'!$B$6</f>
+        <v>0.5</v>
+      </c>
       <c r="U11" s="3">
-        <f>T11/'A Dylan Data'!$B$6</f>
-        <v>0.5</v>
+        <v>72040</v>
       </c>
       <c r="V11" s="3">
-        <v>72040</v>
-      </c>
-      <c r="W11" s="3">
         <f t="shared" si="7"/>
         <v>6.9405885619100507E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12">
         <v>0.72118959100000002</v>
       </c>
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
       <c r="D12" s="3">
         <v>1</v>
       </c>
@@ -1734,79 +1697,76 @@
         <v>1</v>
       </c>
       <c r="F12" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="3">
         <v>1</v>
       </c>
       <c r="I12" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" s="3">
         <v>1</v>
       </c>
       <c r="L12" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M12" s="3">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="N12" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="O12" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P12" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="Q12" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="R12" s="3">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="S12" s="3">
+      <c r="R12" s="3">
         <f t="shared" si="5"/>
         <v>0.625</v>
       </c>
-      <c r="T12" s="3">
+      <c r="S12" s="3">
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
+      <c r="T12" s="3">
+        <f>S12/'A Dylan Data'!$B$6</f>
+        <v>0.7</v>
+      </c>
       <c r="U12" s="3">
-        <f>T12/'A Dylan Data'!$B$6</f>
-        <v>0.7</v>
+        <v>122955</v>
       </c>
       <c r="V12" s="3">
-        <v>122955</v>
-      </c>
-      <c r="W12" s="3">
         <f t="shared" si="7"/>
         <v>5.6931397665812691E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13">
         <v>0.764444444</v>
       </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
       <c r="D13" s="3">
         <v>1</v>
       </c>
@@ -1832,81 +1792,78 @@
         <v>1</v>
       </c>
       <c r="L13" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13" s="3">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="N13" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="O13" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P13" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="Q13" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="R13" s="3">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="S13" s="3">
+      <c r="R13" s="3">
         <f t="shared" si="5"/>
         <v>0.875</v>
       </c>
-      <c r="T13" s="3">
+      <c r="S13" s="3">
         <f t="shared" si="6"/>
         <v>9</v>
       </c>
+      <c r="T13" s="3">
+        <f>S13/'A Dylan Data'!$B$6</f>
+        <v>0.9</v>
+      </c>
       <c r="U13" s="3">
-        <f>T13/'A Dylan Data'!$B$6</f>
-        <v>0.9</v>
+        <v>125311</v>
       </c>
       <c r="V13" s="3">
-        <v>125311</v>
-      </c>
-      <c r="W13" s="3">
         <f t="shared" si="7"/>
         <v>7.1821308584242405E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14">
         <v>0.72815534000000004</v>
       </c>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
       <c r="D14" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14" s="3">
         <v>0</v>
@@ -1915,58 +1872,55 @@
         <v>0</v>
       </c>
       <c r="M14" s="3">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="N14" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="O14" s="3">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="P14" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q14" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="R14" s="3">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="S14" s="3">
+      <c r="R14" s="3">
         <f t="shared" si="5"/>
         <v>0.375</v>
       </c>
-      <c r="T14" s="3">
+      <c r="S14" s="3">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
+      <c r="T14" s="3">
+        <f>S14/'A Dylan Data'!$B$6</f>
+        <v>0.4</v>
+      </c>
       <c r="U14" s="3">
-        <f>T14/'A Dylan Data'!$B$6</f>
-        <v>0.4</v>
+        <v>69219</v>
       </c>
       <c r="V14" s="3">
-        <v>69219</v>
-      </c>
-      <c r="W14" s="3">
         <f t="shared" si="7"/>
         <v>5.7787601670061688E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15">
         <v>0.78749999999999998</v>
       </c>
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
       <c r="D15" s="3">
         <v>1</v>
       </c>
@@ -1989,81 +1943,78 @@
         <v>1</v>
       </c>
       <c r="K15" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15" s="3">
         <v>0</v>
       </c>
       <c r="M15" s="3">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="N15" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="O15" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P15" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="Q15" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="R15" s="3">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="S15" s="3">
+      <c r="R15" s="3">
         <f t="shared" si="5"/>
         <v>0.75</v>
       </c>
-      <c r="T15" s="3">
+      <c r="S15" s="3">
         <f t="shared" si="6"/>
         <v>8</v>
       </c>
+      <c r="T15" s="3">
+        <f>S15/'A Dylan Data'!$B$6</f>
+        <v>0.8</v>
+      </c>
       <c r="U15" s="3">
-        <f>T15/'A Dylan Data'!$B$6</f>
-        <v>0.8</v>
+        <v>104567</v>
       </c>
       <c r="V15" s="3">
-        <v>104567</v>
-      </c>
-      <c r="W15" s="3">
         <f t="shared" si="7"/>
         <v>7.6505972247458573E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16">
         <v>0.73239436599999996</v>
       </c>
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
       <c r="D16" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="3">
         <v>1</v>
       </c>
       <c r="F16" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="3">
         <v>1</v>
       </c>
       <c r="I16" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" s="3">
         <v>0</v>
@@ -2075,60 +2026,57 @@
         <v>0</v>
       </c>
       <c r="M16" s="3">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N16" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O16" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="P16" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="Q16" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="R16" s="3">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="S16" s="3">
+      <c r="R16" s="3">
         <f t="shared" si="5"/>
         <v>0.375</v>
       </c>
-      <c r="T16" s="3">
+      <c r="S16" s="3">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
+      <c r="T16" s="3">
+        <f>S16/'A Dylan Data'!$B$6</f>
+        <v>0.4</v>
+      </c>
       <c r="U16" s="3">
-        <f>T16/'A Dylan Data'!$B$6</f>
-        <v>0.4</v>
+        <v>46135</v>
       </c>
       <c r="V16" s="3">
-        <v>46135</v>
-      </c>
-      <c r="W16" s="3">
         <f t="shared" si="7"/>
         <v>8.6702070011921539E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17">
         <v>0.71</v>
       </c>
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
       <c r="D17" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="3">
         <v>1</v>
@@ -2137,16 +2085,16 @@
         <v>1</v>
       </c>
       <c r="G17" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="3">
         <v>1</v>
       </c>
       <c r="J17" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17" s="3">
         <v>0</v>
@@ -2155,58 +2103,55 @@
         <v>0</v>
       </c>
       <c r="M17" s="3">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N17" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O17" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="P17" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="Q17" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="R17" s="3">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="S17" s="3">
+      <c r="R17" s="3">
         <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
-      <c r="T17" s="3">
+      <c r="S17" s="3">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
+      <c r="T17" s="3">
+        <f>S17/'A Dylan Data'!$B$6</f>
+        <v>0.5</v>
+      </c>
       <c r="U17" s="3">
-        <f>T17/'A Dylan Data'!$B$6</f>
-        <v>0.5</v>
+        <v>54748</v>
       </c>
       <c r="V17" s="3">
-        <v>54748</v>
-      </c>
-      <c r="W17" s="3">
         <f t="shared" si="7"/>
         <v>9.1327537078980059E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18">
         <v>0.688073394</v>
       </c>
+      <c r="C18" s="3">
+        <v>1</v>
+      </c>
       <c r="D18" s="3">
         <v>1</v>
       </c>
@@ -2214,7 +2159,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" s="3">
         <v>0</v>
@@ -2226,67 +2171,64 @@
         <v>0</v>
       </c>
       <c r="J18" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" s="3">
         <v>1</v>
       </c>
       <c r="L18" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M18" s="3">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="N18" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="O18" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P18" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="Q18" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="R18" s="3">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="S18" s="3">
+      <c r="R18" s="3">
         <f t="shared" si="5"/>
         <v>0.375</v>
       </c>
-      <c r="T18" s="3">
+      <c r="S18" s="3">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
+      <c r="T18" s="3">
+        <f>S18/'A Dylan Data'!$B$6</f>
+        <v>0.5</v>
+      </c>
       <c r="U18" s="3">
-        <f>T18/'A Dylan Data'!$B$6</f>
-        <v>0.5</v>
+        <v>69850</v>
       </c>
       <c r="V18" s="3">
-        <v>69850</v>
-      </c>
-      <c r="W18" s="3">
         <f t="shared" si="7"/>
         <v>7.158196134574088E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19">
         <v>0.72180451099999998</v>
       </c>
+      <c r="C19" s="3">
+        <v>1</v>
+      </c>
       <c r="D19" s="3">
         <v>1</v>
       </c>
@@ -2306,7 +2248,7 @@
         <v>1</v>
       </c>
       <c r="J19" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19" s="3">
         <v>0</v>
@@ -2315,50 +2257,47 @@
         <v>0</v>
       </c>
       <c r="M19" s="3">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="N19" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="O19" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P19" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="Q19" s="3">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="R19" s="3">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="S19" s="3">
+      <c r="R19" s="3">
         <f t="shared" si="5"/>
         <v>0.625</v>
       </c>
-      <c r="T19" s="3">
+      <c r="S19" s="3">
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
+      <c r="T19" s="3">
+        <f>S19/'A Dylan Data'!$B$6</f>
+        <v>0.7</v>
+      </c>
       <c r="U19" s="3">
-        <f>T19/'A Dylan Data'!$B$6</f>
-        <v>0.7</v>
+        <v>79989</v>
       </c>
       <c r="V19" s="3">
-        <v>79989</v>
-      </c>
-      <c r="W19" s="3">
         <f t="shared" si="7"/>
         <v>8.7512032904524376E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
+    <row r="21" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -2378,12 +2317,11 @@
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
-      <c r="W21" s="2"/>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A25" s="29"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A25" s="16"/>
       <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
+      <c r="C25" s="29"/>
       <c r="D25" s="29"/>
       <c r="E25" s="29"/>
       <c r="F25" s="29"/>
@@ -2393,7 +2331,7 @@
       <c r="J25" s="29"/>
       <c r="K25" s="29"/>
       <c r="L25" s="29"/>
-      <c r="M25" s="29"/>
+      <c r="M25"/>
       <c r="N25"/>
       <c r="O25"/>
       <c r="P25"/>
@@ -2401,12 +2339,11 @@
       <c r="R25"/>
       <c r="S25"/>
       <c r="T25"/>
-      <c r="U25"/>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A26" s="29"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A26" s="16"/>
       <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
+      <c r="C26" s="29"/>
       <c r="D26" s="29"/>
       <c r="E26" s="29"/>
       <c r="F26" s="29"/>
@@ -2416,7 +2353,7 @@
       <c r="J26" s="29"/>
       <c r="K26" s="29"/>
       <c r="L26" s="29"/>
-      <c r="M26" s="29"/>
+      <c r="M26"/>
       <c r="N26"/>
       <c r="O26"/>
       <c r="P26"/>
@@ -2424,12 +2361,11 @@
       <c r="R26"/>
       <c r="S26"/>
       <c r="T26"/>
-      <c r="U26"/>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A27" s="29"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A27" s="16"/>
       <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
+      <c r="C27" s="29"/>
       <c r="D27" s="29"/>
       <c r="E27" s="29"/>
       <c r="F27" s="29"/>
@@ -2439,7 +2375,7 @@
       <c r="J27" s="29"/>
       <c r="K27" s="29"/>
       <c r="L27" s="29"/>
-      <c r="M27" s="29"/>
+      <c r="M27"/>
       <c r="N27"/>
       <c r="O27"/>
       <c r="P27"/>
@@ -2447,12 +2383,11 @@
       <c r="R27"/>
       <c r="S27"/>
       <c r="T27"/>
-      <c r="U27"/>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A28" s="29"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A28" s="16"/>
       <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
+      <c r="C28" s="29"/>
       <c r="D28" s="29"/>
       <c r="E28" s="29"/>
       <c r="F28" s="29"/>
@@ -2462,7 +2397,7 @@
       <c r="J28" s="29"/>
       <c r="K28" s="29"/>
       <c r="L28" s="29"/>
-      <c r="M28" s="29"/>
+      <c r="M28"/>
       <c r="N28"/>
       <c r="O28"/>
       <c r="P28"/>
@@ -2470,12 +2405,11 @@
       <c r="R28"/>
       <c r="S28"/>
       <c r="T28"/>
-      <c r="U28"/>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A29" s="29"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A29" s="16"/>
       <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
+      <c r="C29" s="29"/>
       <c r="D29" s="29"/>
       <c r="E29" s="29"/>
       <c r="F29" s="29"/>
@@ -2485,7 +2419,7 @@
       <c r="J29" s="29"/>
       <c r="K29" s="29"/>
       <c r="L29" s="29"/>
-      <c r="M29" s="29"/>
+      <c r="M29"/>
       <c r="N29"/>
       <c r="O29"/>
       <c r="P29"/>
@@ -2493,12 +2427,11 @@
       <c r="R29"/>
       <c r="S29"/>
       <c r="T29"/>
-      <c r="U29"/>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A30" s="29"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A30" s="16"/>
       <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
+      <c r="C30" s="29"/>
       <c r="D30" s="29"/>
       <c r="E30" s="29"/>
       <c r="F30" s="29"/>
@@ -2508,7 +2441,7 @@
       <c r="J30" s="29"/>
       <c r="K30" s="29"/>
       <c r="L30" s="29"/>
-      <c r="M30" s="29"/>
+      <c r="M30"/>
       <c r="N30"/>
       <c r="O30"/>
       <c r="P30"/>
@@ -2516,9 +2449,9 @@
       <c r="R30"/>
       <c r="S30"/>
       <c r="T30"/>
-      <c r="U30"/>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="M31"/>
       <c r="N31"/>
       <c r="O31"/>
       <c r="P31"/>
@@ -2526,9 +2459,9 @@
       <c r="R31"/>
       <c r="S31"/>
       <c r="T31"/>
-      <c r="U31"/>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="M32"/>
       <c r="N32"/>
       <c r="O32"/>
       <c r="P32"/>
@@ -2536,7 +2469,6 @@
       <c r="R32"/>
       <c r="S32"/>
       <c r="T32"/>
-      <c r="U32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2569,13 +2501,13 @@
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
       <c r="D1" s="2"/>
       <c r="F1" s="39" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="G1" s="39"/>
       <c r="H1" s="39"/>
@@ -2583,7 +2515,7 @@
       <c r="J1" s="5"/>
       <c r="K1" s="6"/>
       <c r="L1" s="39" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="M1" s="39"/>
       <c r="N1" s="39"/>
@@ -2636,93 +2568,93 @@
         <v>10</v>
       </c>
       <c r="AX1" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1"/>
       <c r="F2" s="8" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="9"/>
       <c r="L2" s="7" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="W2" s="7" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="X2" s="7" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="Y2" s="7" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="Z2" s="7" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="AA2" s="7" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="AB2" s="7" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="AC2" s="7" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="AD2" s="7" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="AM2" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="AN2">
         <v>1</v>
@@ -2752,7 +2684,7 @@
     </row>
     <row r="3" spans="1:50" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="B3" s="10">
         <v>1</v>
@@ -2766,10 +2698,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="I3" s="15"/>
       <c r="J3" s="16"/>
@@ -2821,7 +2753,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="AM3" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="AN3">
         <v>1</v>
@@ -2845,7 +2777,7 @@
     </row>
     <row r="4" spans="1:50" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="30" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="B4" s="30">
         <v>1</v>
@@ -2859,10 +2791,10 @@
         <v>2</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="H4" s="32" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="I4" s="32"/>
       <c r="J4" s="16"/>
@@ -2923,7 +2855,7 @@
       </c>
       <c r="AE4" s="16"/>
       <c r="AM4" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="AO4">
         <v>1</v>
@@ -2947,7 +2879,7 @@
     </row>
     <row r="5" spans="1:50" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="B5" s="19">
         <v>8</v>
@@ -2961,10 +2893,10 @@
         <v>3</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="H5" s="35" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="I5" s="35"/>
       <c r="J5" s="16"/>
@@ -3019,7 +2951,7 @@
       </c>
       <c r="AE5" s="16"/>
       <c r="AM5" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="AO5">
         <v>1</v>
@@ -3040,7 +2972,7 @@
     </row>
     <row r="6" spans="1:50" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="B6" s="7">
         <f>SUM(B3:B5)</f>
@@ -3055,10 +2987,10 @@
         <v>4</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="H6" s="35" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="I6" s="35"/>
       <c r="J6" s="16"/>
@@ -3099,7 +3031,7 @@
       </c>
       <c r="AE6" s="16"/>
       <c r="AM6" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="AN6">
         <v>1</v>
@@ -3139,10 +3071,10 @@
         <v>5</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="H7" s="35" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="I7" s="35"/>
       <c r="J7" s="16"/>
@@ -3195,7 +3127,7 @@
       </c>
       <c r="AE7" s="16"/>
       <c r="AM7" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="AN7">
         <v>1</v>
@@ -3223,10 +3155,10 @@
         <v>6</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="H8" s="35" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="I8" s="35"/>
       <c r="J8" s="16"/>
@@ -3277,7 +3209,7 @@
       </c>
       <c r="AE8" s="16"/>
       <c r="AM8" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="AN8">
         <v>1</v>
@@ -3320,10 +3252,10 @@
         <v>7</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="H9" s="35" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="I9" s="35"/>
       <c r="J9" s="16"/>
@@ -3376,7 +3308,7 @@
       </c>
       <c r="AE9" s="16"/>
       <c r="AM9" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="AN9">
         <v>1</v>
@@ -3413,10 +3345,10 @@
         <v>8</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="H10" s="35" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="I10" s="35"/>
       <c r="J10" s="16"/>
@@ -3465,7 +3397,7 @@
       </c>
       <c r="AE10" s="16"/>
       <c r="AM10" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="AO10">
         <v>1</v>
@@ -3496,10 +3428,10 @@
         <v>9</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="H11" s="35" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="I11" s="35"/>
       <c r="J11" s="16"/>
@@ -3538,7 +3470,7 @@
       </c>
       <c r="AE11" s="16"/>
       <c r="AM11" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="AN11">
         <v>1</v>
@@ -3572,10 +3504,10 @@
         <v>10</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="H12" s="35" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="I12" s="35"/>
       <c r="J12" s="16"/>
@@ -3608,7 +3540,7 @@
       </c>
       <c r="AE12" s="16"/>
       <c r="AM12" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="AN12">
         <v>1</v>
@@ -3638,7 +3570,7 @@
       <c r="I13" s="24"/>
       <c r="J13" s="16"/>
       <c r="K13" s="25" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="L13" s="26">
         <f t="shared" ref="L13:AC13" si="2">(SUM(L3:L12))/10</f>
@@ -3713,11 +3645,11 @@
         <v>0.6</v>
       </c>
       <c r="AD13" s="7" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="AE13" s="16"/>
       <c r="AM13" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="AN13">
         <v>1</v>
@@ -3753,7 +3685,7 @@
       <c r="I14" s="24"/>
       <c r="J14" s="16"/>
       <c r="K14" s="27" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="L14" s="28">
         <f>AVERAGE(L13:AC13)</f>
@@ -3782,7 +3714,7 @@
       </c>
       <c r="AE14" s="16"/>
       <c r="AM14" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="AO14">
         <v>1</v>
@@ -3803,7 +3735,7 @@
     </row>
     <row r="15" spans="1:50" x14ac:dyDescent="0.2">
       <c r="AM15" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="AN15">
         <v>1</v>
@@ -3830,7 +3762,7 @@
     </row>
     <row r="16" spans="1:50" x14ac:dyDescent="0.2">
       <c r="AM16" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="AP16">
         <v>1</v>
@@ -3851,7 +3783,7 @@
     </row>
     <row r="17" spans="39:50" x14ac:dyDescent="0.2">
       <c r="AM17" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="AO17">
         <v>1</v>
@@ -3878,7 +3810,7 @@
     </row>
     <row r="18" spans="39:50" x14ac:dyDescent="0.2">
       <c r="AM18" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="AN18">
         <v>1</v>
@@ -3905,7 +3837,7 @@
     </row>
     <row r="19" spans="39:50" x14ac:dyDescent="0.2">
       <c r="AM19" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="AN19">
         <v>1</v>

</xml_diff>